<commit_message>
updated xls data files
</commit_message>
<xml_diff>
--- a/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/Group1_MRI_data_layer1.xlsx
+++ b/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/Group1_MRI_data_layer1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/anna_canal_garcia_ki_se/Documents/Dokument/GitHub/Braph-2.0-Matlab/braph2/workflows/MultiplexMRI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kise-my.sharepoint.com/personal/anna_canal_garcia_ki_se/Documents/Dokument/GitHub/Braph-2.0-Matlab/braph2/workflows/MultiplexMRI/MultiplexMRI_examples/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_DE5CBECA8F79A8B36A3704F0FB5CC233402F0403" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC60CB84-0ABF-422E-B5DD-9BA0ECFEA773}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_DE5CBECA8F79A8B36A3704F0FB5CC233402F0403" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1BA64D7-7EB5-4CDC-AD7D-E06B6138E357}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -235,7 +235,37 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>notes1</t>
+  </si>
+  <si>
+    <t>notes2</t>
+  </si>
+  <si>
+    <t>notes3</t>
+  </si>
+  <si>
+    <t>notes4</t>
+  </si>
+  <si>
+    <t>notes5</t>
+  </si>
+  <si>
+    <t>notes6</t>
+  </si>
+  <si>
+    <t>notes7</t>
+  </si>
+  <si>
+    <t>notes8</t>
+  </si>
+  <si>
+    <t>notes9</t>
+  </si>
+  <si>
+    <t>notes10</t>
   </si>
 </sst>
 </file>
@@ -646,7 +676,7 @@
   <dimension ref="A1:BS11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -868,13 +898,13 @@
     </row>
     <row r="2" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>0.43000467331988951</v>
@@ -1083,13 +1113,13 @@
     </row>
     <row r="3" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>0.31130251520430008</v>
@@ -1298,13 +1328,13 @@
     </row>
     <row r="4" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D4">
         <v>0.91359318452163385</v>
@@ -1513,13 +1543,13 @@
     </row>
     <row r="5" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>8.1418585823363254E-2</v>
@@ -1728,13 +1758,13 @@
     </row>
     <row r="6" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D6">
         <v>0.46809505230837589</v>
@@ -1943,13 +1973,13 @@
     </row>
     <row r="7" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>0.62042601063254166</v>
@@ -2158,13 +2188,13 @@
     </row>
     <row r="8" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>7.0254307432461296E-3</v>
@@ -2373,13 +2403,13 @@
     </row>
     <row r="9" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D9">
         <v>0.47140076417359378</v>
@@ -2588,13 +2618,13 @@
     </row>
     <row r="10" spans="1:71" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>0.53487850648318458</v>
@@ -2802,14 +2832,14 @@
       </c>
     </row>
     <row r="11" spans="1:71" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <v>9</v>
+      <c r="A11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D11">
         <v>0.63893515600733652</v>

</xml_diff>